<commit_message>
Codigos de matlab y union de dac-adc-tx
</commit_message>
<xml_diff>
--- a/proyectos/19_dac_adc_nval/dac_adc_voltajes.xlsx
+++ b/proyectos/19_dac_adc_nval/dac_adc_voltajes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop_old\proyecto_ubolometro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop_old\proyecto_ubolometro\proyectos\19_dac_adc_nval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D29CA01A-39A2-472E-96D2-2EE5F7335C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B9EC7D-99A8-4F91-A0CC-EBDFB41318F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A4E26C9B-42C0-4A7E-8221-10182986009A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A4E26C9B-42C0-4A7E-8221-10182986009A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>Voltaje</t>
   </si>
@@ -93,6 +93,30 @@
   </si>
   <si>
     <t>Voltaje recibido</t>
+  </si>
+  <si>
+    <t>Código: dac_adc_1val</t>
+  </si>
+  <si>
+    <t>Código: dac_adc_nval</t>
+  </si>
+  <si>
+    <t>Valor Binario</t>
+  </si>
+  <si>
+    <t>1001 1011 0010</t>
+  </si>
+  <si>
+    <t>0111 1100 0001</t>
+  </si>
+  <si>
+    <t>0010 0110 1100</t>
+  </si>
+  <si>
+    <t>0111 1100 0010</t>
+  </si>
+  <si>
+    <t>1001 1011 0011</t>
   </si>
 </sst>
 </file>
@@ -154,7 +178,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -307,79 +331,119 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,10 +778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87F7E0A-7755-42D9-9640-32763B91400C}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,326 +790,574 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="15" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="17"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="19"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
+      <c r="C3" s="20"/>
+      <c r="D3" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="13" t="s">
+      <c r="E3" s="21"/>
+      <c r="F3" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
+      <c r="G3" s="20"/>
+      <c r="H3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3" t="s">
+      <c r="I3" s="20"/>
+      <c r="J3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <f>(3.3/4095)*B3</f>
+      <c r="K3" s="21"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <f>(3.3/4095)*B4</f>
         <v>0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B4" s="12">
         <v>0</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+      <c r="C4" s="12"/>
+      <c r="D4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="13" t="s">
+      <c r="E4" s="11"/>
+      <c r="F4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3">
+      <c r="G4" s="23"/>
+      <c r="H4" s="12">
         <v>16</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3">
-        <f>(3.3/4095)*H3</f>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12">
+        <f>(3.3/4095)*H4</f>
         <v>1.2893772893772894E-2</v>
       </c>
-      <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <f>(3.3/4095)*B4</f>
+      <c r="K4" s="11"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <f>(3.3/4095)*B5</f>
         <v>0.66</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B5" s="12">
         <v>819</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="13" t="s">
+      <c r="E5" s="11"/>
+      <c r="F5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3">
+      <c r="G5" s="23"/>
+      <c r="H5" s="12">
         <v>816</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3">
-        <f t="shared" ref="J4:J8" si="0">(3.3/4095)*H4</f>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12">
+        <f t="shared" ref="J5:J9" si="0">(3.3/4095)*H5</f>
         <v>0.65758241758241753</v>
       </c>
-      <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <f t="shared" ref="A5:A8" si="1">(3.3/4095)*B5</f>
+      <c r="K5" s="11"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <f t="shared" ref="A6:A9" si="1">(3.3/4095)*B6</f>
         <v>1.32</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B6" s="12">
         <v>1638</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
+      <c r="C6" s="12"/>
+      <c r="D6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="13" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3">
+      <c r="G6" s="23"/>
+      <c r="H6" s="12">
         <v>1637</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3">
+      <c r="I6" s="12"/>
+      <c r="J6" s="12">
         <f t="shared" si="0"/>
         <v>1.3191941391941393</v>
       </c>
-      <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="K6" s="11"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <f t="shared" si="1"/>
         <v>1.98</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B7" s="12">
         <v>2457</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
+      <c r="C7" s="12"/>
+      <c r="D7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="13" t="s">
+      <c r="E7" s="11"/>
+      <c r="F7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3">
+      <c r="G7" s="23"/>
+      <c r="H7" s="12">
         <v>2456</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3">
+      <c r="I7" s="12"/>
+      <c r="J7" s="12">
         <f t="shared" si="0"/>
         <v>1.9791941391941392</v>
       </c>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="K7" s="11"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <f t="shared" si="1"/>
         <v>2.64</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B8" s="12">
         <v>3276</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
+      <c r="C8" s="12"/>
+      <c r="D8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="13" t="s">
+      <c r="E8" s="11"/>
+      <c r="F8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3">
+      <c r="G8" s="23"/>
+      <c r="H8" s="12">
         <v>3273</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3">
+      <c r="I8" s="12"/>
+      <c r="J8" s="12">
         <f t="shared" si="0"/>
         <v>2.6375824175824176</v>
       </c>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="K8" s="11"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <f t="shared" si="1"/>
         <v>3.3</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B9" s="13">
         <v>4095</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8" t="s">
+      <c r="C9" s="13"/>
+      <c r="D9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="14" t="s">
+      <c r="E9" s="8"/>
+      <c r="F9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8">
+      <c r="G9" s="13"/>
+      <c r="H9" s="13">
         <v>4091</v>
       </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8">
+      <c r="I9" s="13"/>
+      <c r="J9" s="13">
         <f t="shared" si="0"/>
         <v>3.2967765567765568</v>
       </c>
-      <c r="K8" s="9"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="K9" s="8"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B11" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="22"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="19">
+      <c r="C11" s="33"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
         <v>0</v>
       </c>
-      <c r="B11" s="13">
-        <f>J3</f>
+      <c r="B12" s="10">
+        <f>J4</f>
         <v>1.2893772893772894E-2</v>
       </c>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
+      <c r="C12" s="11"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>0.66</v>
       </c>
-      <c r="B12" s="13">
-        <f t="shared" ref="B12:B16" si="2">J4</f>
+      <c r="B13" s="10">
+        <f>J5</f>
         <v>0.65758241758241753</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="F12" s="23"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="19">
+      <c r="C13" s="11"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
         <v>1.32</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B14" s="10">
+        <f>J6</f>
+        <v>1.3191941391941393</v>
+      </c>
+      <c r="C14" s="11"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>1.98</v>
+      </c>
+      <c r="B15" s="10">
+        <f>J7</f>
+        <v>1.9791941391941392</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>2.64</v>
+      </c>
+      <c r="B16" s="10">
+        <f>J8</f>
+        <v>2.6375824175824176</v>
+      </c>
+      <c r="C16" s="11"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>3.3</v>
+      </c>
+      <c r="B17" s="7">
+        <f>J9</f>
+        <v>3.2967765567765568</v>
+      </c>
+      <c r="C17" s="8"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="30"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="K21" s="11"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <f>(3.3/4095)*B22</f>
+        <v>0.49963369963369964</v>
+      </c>
+      <c r="B22" s="23">
+        <v>620</v>
+      </c>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23">
+        <v>620</v>
+      </c>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23">
+        <f>(3.3/4095)*H22</f>
+        <v>0.49963369963369964</v>
+      </c>
+      <c r="K22" s="11"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <f t="shared" ref="A23:A25" si="2">(3.3/4095)*B23</f>
+        <v>1.5996336996336997</v>
+      </c>
+      <c r="B23" s="23">
+        <v>1985</v>
+      </c>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23">
+        <v>1986</v>
+      </c>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23">
+        <f t="shared" ref="J23:J25" si="3">(3.3/4095)*H23</f>
+        <v>1.6004395604395605</v>
+      </c>
+      <c r="K23" s="11"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <f t="shared" si="2"/>
-        <v>1.3191941391941393</v>
-      </c>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
-        <v>1.98</v>
-      </c>
-      <c r="B14" s="13">
+        <v>2.0001465201465201</v>
+      </c>
+      <c r="B24" s="23">
+        <v>2482</v>
+      </c>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23">
+        <v>2483</v>
+      </c>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23">
+        <f t="shared" si="3"/>
+        <v>2.000952380952381</v>
+      </c>
+      <c r="K24" s="11"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
         <f t="shared" si="2"/>
-        <v>1.9791941391941392</v>
-      </c>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
-        <v>2.64</v>
-      </c>
-      <c r="B15" s="13">
-        <f t="shared" si="2"/>
-        <v>2.6375824175824176</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="23"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="20">
         <v>3.3</v>
       </c>
-      <c r="B16" s="14">
-        <f t="shared" si="2"/>
-        <v>3.2967765567765568</v>
-      </c>
-      <c r="C16" s="9"/>
+      <c r="B25" s="13">
+        <v>4095</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13">
+        <v>4095</v>
+      </c>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13">
+        <f t="shared" si="3"/>
+        <v>3.3</v>
+      </c>
+      <c r="K25" s="8"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="9"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <f>A22</f>
+        <v>0.49963369963369964</v>
+      </c>
+      <c r="B28" s="23">
+        <f>J22</f>
+        <v>0.49963369963369964</v>
+      </c>
+      <c r="C28" s="11"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <f t="shared" ref="A29:A31" si="4">A23</f>
+        <v>1.5996336996336997</v>
+      </c>
+      <c r="B29" s="23">
+        <f t="shared" ref="B29:B31" si="5">J23</f>
+        <v>1.6004395604395605</v>
+      </c>
+      <c r="C29" s="11"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <f t="shared" si="4"/>
+        <v>2.0001465201465201</v>
+      </c>
+      <c r="B30" s="23">
+        <f t="shared" si="5"/>
+        <v>2.000952380952381</v>
+      </c>
+      <c r="C30" s="11"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <f t="shared" si="4"/>
+        <v>3.3</v>
+      </c>
+      <c r="B31" s="13">
+        <f t="shared" si="5"/>
+        <v>3.3</v>
+      </c>
+      <c r="C31" s="8"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
+  <mergeCells count="76">
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="F20:K20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="H8:I8"/>
-    <mergeCell ref="J2:K2"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="J8:K8"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>